<commit_message>
grouping cluster result in perhitungan/views.py
</commit_message>
<xml_diff>
--- a/static/files/rm/rm.xlsx
+++ b/static/files/rm/rm.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dokumen Kuliah\Skripsi Binus\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3525B83-A7D9-45D0-8F01-FFE46B674B8C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BDEF0E4-9D30-488A-9FA3-CE1A7FE9EE0D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="84">
   <si>
     <t>nama_pasien</t>
   </si>
@@ -116,6 +116,162 @@
   </si>
   <si>
     <t>K10 B70</t>
+  </si>
+  <si>
+    <t>Pasien G</t>
+  </si>
+  <si>
+    <t>Pasien H</t>
+  </si>
+  <si>
+    <t>Pasien I</t>
+  </si>
+  <si>
+    <t>Pasien J</t>
+  </si>
+  <si>
+    <t>Pasien K</t>
+  </si>
+  <si>
+    <t>Pasien L</t>
+  </si>
+  <si>
+    <t>Pasien M</t>
+  </si>
+  <si>
+    <t>Pasien N</t>
+  </si>
+  <si>
+    <t>Pasien O</t>
+  </si>
+  <si>
+    <t>Pasien P</t>
+  </si>
+  <si>
+    <t>Pasien Q</t>
+  </si>
+  <si>
+    <t>Pasien R</t>
+  </si>
+  <si>
+    <t>Pasien S</t>
+  </si>
+  <si>
+    <t>Pasien T</t>
+  </si>
+  <si>
+    <t>Pasien U</t>
+  </si>
+  <si>
+    <t>Pasien V</t>
+  </si>
+  <si>
+    <t>Pasien W</t>
+  </si>
+  <si>
+    <t>Pasien X</t>
+  </si>
+  <si>
+    <t>Pasien Y</t>
+  </si>
+  <si>
+    <t>Pasien Z</t>
+  </si>
+  <si>
+    <t>Pasien AA</t>
+  </si>
+  <si>
+    <t>Pasien AB</t>
+  </si>
+  <si>
+    <t>Pasien AC</t>
+  </si>
+  <si>
+    <t>I</t>
+  </si>
+  <si>
+    <t>J</t>
+  </si>
+  <si>
+    <t>K</t>
+  </si>
+  <si>
+    <t>M</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>O</t>
+  </si>
+  <si>
+    <t>Q</t>
+  </si>
+  <si>
+    <t>R</t>
+  </si>
+  <si>
+    <t>S</t>
+  </si>
+  <si>
+    <t>T</t>
+  </si>
+  <si>
+    <t>U</t>
+  </si>
+  <si>
+    <t>V</t>
+  </si>
+  <si>
+    <t>W</t>
+  </si>
+  <si>
+    <t>Sakit_Gigi</t>
+  </si>
+  <si>
+    <t>G40</t>
+  </si>
+  <si>
+    <t>DBD</t>
+  </si>
+  <si>
+    <t>C10</t>
+  </si>
+  <si>
+    <t>Demam DBD</t>
+  </si>
+  <si>
+    <t>B70 C10</t>
+  </si>
+  <si>
+    <t>Gastritis</t>
+  </si>
+  <si>
+    <t>K29</t>
+  </si>
+  <si>
+    <t>Anemia Gastritis</t>
+  </si>
+  <si>
+    <t>D50 K29</t>
+  </si>
+  <si>
+    <t>Demam Gastritis</t>
+  </si>
+  <si>
+    <t>B70 K29</t>
+  </si>
+  <si>
+    <t>Demam Sakit_Kepala</t>
+  </si>
+  <si>
+    <t>B70 G30</t>
+  </si>
+  <si>
+    <t>Sakit_Gigi Demam</t>
+  </si>
+  <si>
+    <t>G40  B70</t>
   </si>
 </sst>
 </file>
@@ -956,15 +1112,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F7"/>
+  <dimension ref="A1:F30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="F24" sqref="F24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="5" max="5" width="14.7109375" customWidth="1"/>
+    <col min="5" max="5" width="18.28515625" customWidth="1"/>
     <col min="6" max="6" width="21.5703125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1002,10 +1158,10 @@
         <v>5</v>
       </c>
       <c r="E2" t="s">
-        <v>13</v>
+        <v>78</v>
       </c>
       <c r="F2" t="s">
-        <v>17</v>
+        <v>79</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -1076,7 +1232,7 @@
         <v>4</v>
       </c>
       <c r="C6">
-        <v>65</v>
+        <v>25</v>
       </c>
       <c r="D6" t="s">
         <v>12</v>
@@ -1106,6 +1262,466 @@
       </c>
       <c r="F7" t="s">
         <v>30</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>32</v>
+      </c>
+      <c r="B8" t="s">
+        <v>4</v>
+      </c>
+      <c r="C8">
+        <v>18</v>
+      </c>
+      <c r="D8" t="s">
+        <v>5</v>
+      </c>
+      <c r="E8" t="s">
+        <v>13</v>
+      </c>
+      <c r="F8" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>33</v>
+      </c>
+      <c r="B9" t="s">
+        <v>6</v>
+      </c>
+      <c r="C9">
+        <v>41</v>
+      </c>
+      <c r="D9" t="s">
+        <v>7</v>
+      </c>
+      <c r="E9" t="s">
+        <v>24</v>
+      </c>
+      <c r="F9" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>34</v>
+      </c>
+      <c r="B10" t="s">
+        <v>6</v>
+      </c>
+      <c r="C10">
+        <v>23</v>
+      </c>
+      <c r="D10" t="s">
+        <v>8</v>
+      </c>
+      <c r="E10" t="s">
+        <v>26</v>
+      </c>
+      <c r="F10" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>35</v>
+      </c>
+      <c r="B11" t="s">
+        <v>6</v>
+      </c>
+      <c r="C11">
+        <v>55</v>
+      </c>
+      <c r="D11" t="s">
+        <v>9</v>
+      </c>
+      <c r="E11" t="s">
+        <v>25</v>
+      </c>
+      <c r="F11" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>36</v>
+      </c>
+      <c r="B12" t="s">
+        <v>4</v>
+      </c>
+      <c r="C12">
+        <v>2</v>
+      </c>
+      <c r="D12" t="s">
+        <v>12</v>
+      </c>
+      <c r="E12" t="s">
+        <v>14</v>
+      </c>
+      <c r="F12" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>37</v>
+      </c>
+      <c r="B13" t="s">
+        <v>6</v>
+      </c>
+      <c r="C13">
+        <v>38</v>
+      </c>
+      <c r="D13" t="s">
+        <v>28</v>
+      </c>
+      <c r="E13" t="s">
+        <v>29</v>
+      </c>
+      <c r="F13" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>38</v>
+      </c>
+      <c r="B14" t="s">
+        <v>4</v>
+      </c>
+      <c r="C14">
+        <v>34</v>
+      </c>
+      <c r="D14" t="s">
+        <v>55</v>
+      </c>
+      <c r="E14" t="s">
+        <v>13</v>
+      </c>
+      <c r="F14" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>39</v>
+      </c>
+      <c r="B15" t="s">
+        <v>6</v>
+      </c>
+      <c r="C15">
+        <v>56</v>
+      </c>
+      <c r="D15" t="s">
+        <v>56</v>
+      </c>
+      <c r="E15" t="s">
+        <v>24</v>
+      </c>
+      <c r="F15" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>40</v>
+      </c>
+      <c r="B16" t="s">
+        <v>4</v>
+      </c>
+      <c r="C16">
+        <v>71</v>
+      </c>
+      <c r="D16" t="s">
+        <v>57</v>
+      </c>
+      <c r="E16" t="s">
+        <v>72</v>
+      </c>
+      <c r="F16" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>41</v>
+      </c>
+      <c r="B17" t="s">
+        <v>6</v>
+      </c>
+      <c r="C17">
+        <v>23</v>
+      </c>
+      <c r="D17" t="s">
+        <v>4</v>
+      </c>
+      <c r="E17" t="s">
+        <v>70</v>
+      </c>
+      <c r="F17" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>42</v>
+      </c>
+      <c r="B18" t="s">
+        <v>4</v>
+      </c>
+      <c r="C18">
+        <v>11</v>
+      </c>
+      <c r="D18" t="s">
+        <v>58</v>
+      </c>
+      <c r="E18" t="s">
+        <v>25</v>
+      </c>
+      <c r="F18" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>43</v>
+      </c>
+      <c r="B19" t="s">
+        <v>4</v>
+      </c>
+      <c r="C19">
+        <v>0.5</v>
+      </c>
+      <c r="D19" t="s">
+        <v>59</v>
+      </c>
+      <c r="E19" t="s">
+        <v>14</v>
+      </c>
+      <c r="F19" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>44</v>
+      </c>
+      <c r="B20" t="s">
+        <v>4</v>
+      </c>
+      <c r="C20">
+        <v>28</v>
+      </c>
+      <c r="D20" t="s">
+        <v>60</v>
+      </c>
+      <c r="E20" t="s">
+        <v>76</v>
+      </c>
+      <c r="F20" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>45</v>
+      </c>
+      <c r="B21" t="s">
+        <v>6</v>
+      </c>
+      <c r="C21">
+        <v>39</v>
+      </c>
+      <c r="D21" t="s">
+        <v>6</v>
+      </c>
+      <c r="E21" t="s">
+        <v>82</v>
+      </c>
+      <c r="F21" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>46</v>
+      </c>
+      <c r="B22" t="s">
+        <v>6</v>
+      </c>
+      <c r="C22">
+        <v>45</v>
+      </c>
+      <c r="D22" t="s">
+        <v>61</v>
+      </c>
+      <c r="E22" t="s">
+        <v>74</v>
+      </c>
+      <c r="F22" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>47</v>
+      </c>
+      <c r="B23" t="s">
+        <v>4</v>
+      </c>
+      <c r="C23">
+        <v>51</v>
+      </c>
+      <c r="D23" t="s">
+        <v>62</v>
+      </c>
+      <c r="E23" t="s">
+        <v>13</v>
+      </c>
+      <c r="F23" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>48</v>
+      </c>
+      <c r="B24" t="s">
+        <v>4</v>
+      </c>
+      <c r="C24">
+        <v>12</v>
+      </c>
+      <c r="D24" t="s">
+        <v>63</v>
+      </c>
+      <c r="E24" t="s">
+        <v>24</v>
+      </c>
+      <c r="F24" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>49</v>
+      </c>
+      <c r="B25" t="s">
+        <v>4</v>
+      </c>
+      <c r="C25">
+        <v>18</v>
+      </c>
+      <c r="D25" t="s">
+        <v>64</v>
+      </c>
+      <c r="E25" t="s">
+        <v>76</v>
+      </c>
+      <c r="F25" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>50</v>
+      </c>
+      <c r="B26" t="s">
+        <v>6</v>
+      </c>
+      <c r="C26">
+        <v>48</v>
+      </c>
+      <c r="D26" t="s">
+        <v>65</v>
+      </c>
+      <c r="E26" t="s">
+        <v>80</v>
+      </c>
+      <c r="F26" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>51</v>
+      </c>
+      <c r="B27" t="s">
+        <v>4</v>
+      </c>
+      <c r="C27">
+        <v>21</v>
+      </c>
+      <c r="D27" t="s">
+        <v>66</v>
+      </c>
+      <c r="E27" t="s">
+        <v>24</v>
+      </c>
+      <c r="F27" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>52</v>
+      </c>
+      <c r="B28" t="s">
+        <v>6</v>
+      </c>
+      <c r="C28">
+        <v>75</v>
+      </c>
+      <c r="D28" t="s">
+        <v>67</v>
+      </c>
+      <c r="E28" t="s">
+        <v>26</v>
+      </c>
+      <c r="F28" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>53</v>
+      </c>
+      <c r="B29" t="s">
+        <v>4</v>
+      </c>
+      <c r="C29">
+        <v>63</v>
+      </c>
+      <c r="D29" t="s">
+        <v>8</v>
+      </c>
+      <c r="E29" t="s">
+        <v>25</v>
+      </c>
+      <c r="F29" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>54</v>
+      </c>
+      <c r="B30" t="s">
+        <v>6</v>
+      </c>
+      <c r="C30">
+        <v>58</v>
+      </c>
+      <c r="D30" t="s">
+        <v>9</v>
+      </c>
+      <c r="E30" t="s">
+        <v>68</v>
+      </c>
+      <c r="F30" t="s">
+        <v>69</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add stop iteration function if centroid doesn't changes anymore
</commit_message>
<xml_diff>
--- a/static/files/rm/rm.xlsx
+++ b/static/files/rm/rm.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dokumen Kuliah\Skripsi Binus\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BDEF0E4-9D30-488A-9FA3-CE1A7FE9EE0D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05927BC8-DB7E-4DCC-92DD-2C60CBC95B21}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="108">
   <si>
     <t>nama_pasien</t>
   </si>
@@ -272,6 +272,78 @@
   </si>
   <si>
     <t>G40  B70</t>
+  </si>
+  <si>
+    <t>Pasien AD</t>
+  </si>
+  <si>
+    <t>Pasien AE</t>
+  </si>
+  <si>
+    <t>Pasien AF</t>
+  </si>
+  <si>
+    <t>Pasien AG</t>
+  </si>
+  <si>
+    <t>Pasien AH</t>
+  </si>
+  <si>
+    <t>Pasien AJ</t>
+  </si>
+  <si>
+    <t>Pasien AK</t>
+  </si>
+  <si>
+    <t>Pasien AL</t>
+  </si>
+  <si>
+    <t>Pasien AM</t>
+  </si>
+  <si>
+    <t>Pasien AN</t>
+  </si>
+  <si>
+    <t>Malaria</t>
+  </si>
+  <si>
+    <t>C12</t>
+  </si>
+  <si>
+    <t>Gerd</t>
+  </si>
+  <si>
+    <t>K31</t>
+  </si>
+  <si>
+    <t>Demam Malaria</t>
+  </si>
+  <si>
+    <t>B70 C12</t>
+  </si>
+  <si>
+    <t>Sakit_Kepala Gerd</t>
+  </si>
+  <si>
+    <t>G30 K31</t>
+  </si>
+  <si>
+    <t>Malaria Sakit_Pinggang</t>
+  </si>
+  <si>
+    <t>C12 G20</t>
+  </si>
+  <si>
+    <t>Sakit_Kepala Anemia</t>
+  </si>
+  <si>
+    <t>G30 D50</t>
+  </si>
+  <si>
+    <t>Diare Demam DBD</t>
+  </si>
+  <si>
+    <t>K10 B70 C10</t>
   </si>
 </sst>
 </file>
@@ -1112,10 +1184,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F30"/>
+  <dimension ref="A1:F40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F24" sqref="F24"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1318,10 +1390,10 @@
         <v>8</v>
       </c>
       <c r="E10" t="s">
-        <v>26</v>
+        <v>106</v>
       </c>
       <c r="F10" t="s">
-        <v>31</v>
+        <v>107</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
@@ -1398,10 +1470,10 @@
         <v>55</v>
       </c>
       <c r="E14" t="s">
-        <v>13</v>
+        <v>98</v>
       </c>
       <c r="F14" t="s">
-        <v>17</v>
+        <v>99</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
@@ -1418,10 +1490,10 @@
         <v>56</v>
       </c>
       <c r="E15" t="s">
-        <v>24</v>
+        <v>104</v>
       </c>
       <c r="F15" t="s">
-        <v>18</v>
+        <v>105</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
@@ -1722,6 +1794,176 @@
       </c>
       <c r="F30" t="s">
         <v>69</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>84</v>
+      </c>
+      <c r="B31" t="s">
+        <v>6</v>
+      </c>
+      <c r="C31">
+        <v>10</v>
+      </c>
+      <c r="E31" t="s">
+        <v>94</v>
+      </c>
+      <c r="F31" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>85</v>
+      </c>
+      <c r="B32" t="s">
+        <v>6</v>
+      </c>
+      <c r="C32">
+        <v>44</v>
+      </c>
+      <c r="E32" t="s">
+        <v>94</v>
+      </c>
+      <c r="F32" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>86</v>
+      </c>
+      <c r="B33" t="s">
+        <v>6</v>
+      </c>
+      <c r="C33">
+        <v>22</v>
+      </c>
+      <c r="E33" t="s">
+        <v>24</v>
+      </c>
+      <c r="F33" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>87</v>
+      </c>
+      <c r="B34" t="s">
+        <v>4</v>
+      </c>
+      <c r="C34">
+        <v>27</v>
+      </c>
+      <c r="E34" t="s">
+        <v>26</v>
+      </c>
+      <c r="F34" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>88</v>
+      </c>
+      <c r="B35" t="s">
+        <v>6</v>
+      </c>
+      <c r="C35">
+        <v>38</v>
+      </c>
+      <c r="E35" t="s">
+        <v>25</v>
+      </c>
+      <c r="F35" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>89</v>
+      </c>
+      <c r="B36" t="s">
+        <v>6</v>
+      </c>
+      <c r="C36">
+        <v>42</v>
+      </c>
+      <c r="E36" t="s">
+        <v>96</v>
+      </c>
+      <c r="F36" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>90</v>
+      </c>
+      <c r="B37" t="s">
+        <v>4</v>
+      </c>
+      <c r="C37">
+        <v>21</v>
+      </c>
+      <c r="E37" t="s">
+        <v>102</v>
+      </c>
+      <c r="F37" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>91</v>
+      </c>
+      <c r="B38" t="s">
+        <v>4</v>
+      </c>
+      <c r="C38">
+        <v>60</v>
+      </c>
+      <c r="E38" t="s">
+        <v>96</v>
+      </c>
+      <c r="F38" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>92</v>
+      </c>
+      <c r="B39" t="s">
+        <v>4</v>
+      </c>
+      <c r="C39">
+        <v>65</v>
+      </c>
+      <c r="E39" t="s">
+        <v>13</v>
+      </c>
+      <c r="F39" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>93</v>
+      </c>
+      <c r="B40" t="s">
+        <v>4</v>
+      </c>
+      <c r="C40">
+        <v>34</v>
+      </c>
+      <c r="E40" t="s">
+        <v>100</v>
+      </c>
+      <c r="F40" t="s">
+        <v>101</v>
       </c>
     </row>
   </sheetData>

</xml_diff>